<commit_message>
udpated the task and forms
</commit_message>
<xml_diff>
--- a/config-nssd-migration-perinatal_workflow/forms/app/psupp_home_visit.xlsx
+++ b/config-nssd-migration-perinatal_workflow/forms/app/psupp_home_visit.xlsx
@@ -360,7 +360,7 @@
     <t>PSuPP Form</t>
   </si>
   <si>
-    <t>psupp_form</t>
+    <t>psupp_home_visit</t>
   </si>
   <si>
     <t>pages</t>
@@ -568,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -667,6 +667,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -1802,10 +1805,10 @@
       <c r="A2" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="34">
         <v>1.0</v>
       </c>
       <c r="D2" s="30" t="s">
@@ -1823,10 +1826,10 @@
       <c r="A3" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="34">
         <v>1.0</v>
       </c>
       <c r="D3" s="30" t="s">

</xml_diff>

<commit_message>
updated the home visit form
</commit_message>
<xml_diff>
--- a/config-nssd-migration-perinatal_workflow/forms/app/psupp_home_visit.xlsx
+++ b/config-nssd-migration-perinatal_workflow/forms/app/psupp_home_visit.xlsx
@@ -357,7 +357,7 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>PSuPP Form</t>
+    <t>PSuPP Home visit</t>
   </si>
   <si>
     <t>psupp_home_visit</t>
@@ -375,15 +375,15 @@
     <r>
       <rPr>
         <rFont val="Cambria"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t xml:space="preserve">PSuPP </t>
+      <t xml:space="preserve">PSuPP Home </t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
       <t>फारम</t>
@@ -1802,7 +1802,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="33" t="s">
         <v>92</v>
       </c>
       <c r="B2" s="33" t="s">
@@ -1823,7 +1823,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="33" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="33" t="s">

</xml_diff>

<commit_message>
debugged and updated the form
</commit_message>
<xml_diff>
--- a/config-nssd-migration-perinatal_workflow/forms/app/psupp_home_visit.xlsx
+++ b/config-nssd-migration-perinatal_workflow/forms/app/psupp_home_visit.xlsx
@@ -201,7 +201,7 @@
     <t xml:space="preserve"> First home visit </t>
   </si>
   <si>
-    <t>${home_visit} ='1'</t>
+    <t>${home_visit} ='visit_1'</t>
   </si>
   <si>
     <t xml:space="preserve">text </t>
@@ -266,7 +266,7 @@
     <t>Second Home Visit</t>
   </si>
   <si>
-    <t>${home_visit} ='2'</t>
+    <t>${home_visit} ='visit_2'</t>
   </si>
   <si>
     <t>text</t>

</xml_diff>